<commit_message>
Added Jumping on Clouds and *linked to educative project
</commit_message>
<xml_diff>
--- a/CountingValleys/CountingValleys.xlsx
+++ b/CountingValleys/CountingValleys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpeddle\source\repos\CAPeddle\HackerRank\CountingValleys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25A04AEE-5207-4466-942C-14389539AAFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8AE2EC-7975-4B28-A6E5-66F18E23F059}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11325" xr2:uid="{03967D5B-BF09-46C2-B3DE-ABBBBA46CA1D}"/>
+    <workbookView xWindow="30750" yWindow="4440" windowWidth="21600" windowHeight="11325" xr2:uid="{03967D5B-BF09-46C2-B3DE-ABBBBA46CA1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="5">
   <si>
     <t>D</t>
   </si>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D585A5FE-CC84-47D9-84E5-ACD1C9C19A24}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B16" sqref="B16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -601,6 +601,102 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:13">
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="G14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>8</v>
+      </c>
+      <c r="J17">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>